<commit_message>
Decision Table issue fix changes
</commit_message>
<xml_diff>
--- a/Spring-Drools/src/main/resources/rules/dtable.xlsx
+++ b/Spring-Drools/src/main/resources/rules/dtable.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>RuleSet</t>
   </si>
@@ -43,98 +43,64 @@
     <t>bankName==$param</t>
   </si>
   <si>
-    <t>durationInYear&gt;= $1,durationInYear&lt;$2</t>
-  </si>
-  <si>
-    <t>fdObject.setFixeddepositInterestRate($param)</t>
+    <t>fdObject.setFixeddepositInterestRate($param);</t>
   </si>
   <si>
     <t>bankName</t>
   </si>
   <si>
-    <t>durationInYear</t>
-  </si>
-  <si>
     <t>set FD Intrest rate</t>
   </si>
   <si>
-    <t>CITI - More than or equal to 1 year and less than 2 years</t>
+    <t>CITI - IntrestRate on Fixed Deposits</t>
   </si>
   <si>
     <t>"CITI"</t>
   </si>
   <si>
-    <t>1,2</t>
-  </si>
-  <si>
     <t>"3%"</t>
   </si>
   <si>
-    <t>CITI - More than or equal to 2 years and less than 3 years</t>
-  </si>
-  <si>
-    <t>2,3</t>
+    <t>ICICI -  IntrestRate on Fixed Deposits</t>
+  </si>
+  <si>
+    <t>"ICICI"</t>
   </si>
   <si>
     <t>"5%"</t>
   </si>
   <si>
-    <t>ICICI - More than or equal to 1 year and less than 2 years</t>
-  </si>
-  <si>
-    <t>"ICICI"</t>
+    <t>HDFC -  IntrestRate on Fixed Deposits</t>
+  </si>
+  <si>
+    <t>"HDFC"</t>
   </si>
   <si>
     <t>"4%"</t>
-  </si>
-  <si>
-    <t>ICICI - More than or equal to 2 year and less than 3 years</t>
-  </si>
-  <si>
-    <t>"6%"</t>
-  </si>
-  <si>
-    <t>HDFC - More than or equal to 1 year and less than 2 years</t>
-  </si>
-  <si>
-    <t>"HDFC"</t>
-  </si>
-  <si>
-    <t>HDFC - More than or equal to 2 year and less than 3 years</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
+    <font/>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -151,9 +117,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -374,8 +337,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="50.57"/>
     <col customWidth="1" min="2" max="2" width="49.29"/>
-    <col customWidth="1" min="3" max="3" width="35.0"/>
-    <col customWidth="1" min="4" max="4" width="32.43"/>
+    <col customWidth="1" min="3" max="3" width="32.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -387,7 +349,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -400,16 +362,13 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -419,112 +378,55 @@
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="s">
+    <row r="12">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>